<commit_message>
Different format for double-checked literature
</commit_message>
<xml_diff>
--- a/data/Literatur_uebersicht.xlsx
+++ b/data/Literatur_uebersicht.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24020"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="1117" documentId="11_3A91CAE99B495269A6C75D2EF1D7B238247307F4" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{16C1E9B4-9AF6-43A0-B13B-2AF98F510066}"/>
+  <xr:revisionPtr revIDLastSave="1119" documentId="11_3A91CAE99B495269A6C75D2EF1D7B238247307F4" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{22AD4EBC-A21F-40E2-8A9E-B81B1A3F3940}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -577,14 +577,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -625,17 +622,8 @@
     <xf numFmtId="2" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="2" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="5" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -643,9 +631,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -1009,10 +1000,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AK7"/>
+  <dimension ref="A1:AH7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
-      <selection activeCell="AH6" sqref="AH6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P4" sqref="A1:AH7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1026,747 +1017,746 @@
     <col min="12" max="12" width="15.42578125" customWidth="1"/>
     <col min="13" max="13" width="27.5703125" style="1" customWidth="1"/>
     <col min="14" max="14" width="16.28515625" style="1" customWidth="1"/>
-    <col min="15" max="17" width="12.85546875" style="1" customWidth="1"/>
-    <col min="18" max="18" width="19" customWidth="1"/>
-    <col min="19" max="19" width="21.28515625" customWidth="1"/>
-    <col min="20" max="20" width="13.42578125" style="25" customWidth="1"/>
-    <col min="21" max="22" width="16.140625" customWidth="1"/>
-    <col min="23" max="24" width="27.42578125" customWidth="1"/>
-    <col min="25" max="26" width="18.42578125" customWidth="1"/>
-    <col min="27" max="28" width="12.28515625" customWidth="1"/>
-    <col min="29" max="30" width="20.28515625" customWidth="1"/>
-    <col min="31" max="31" width="15.140625" style="15" customWidth="1"/>
-    <col min="32" max="32" width="12.140625" style="15" customWidth="1"/>
-    <col min="33" max="33" width="14.42578125" customWidth="1"/>
-    <col min="34" max="34" width="17.42578125" customWidth="1"/>
-    <col min="35" max="35" width="13.28515625" customWidth="1"/>
+    <col min="15" max="15" width="12.85546875" style="1" customWidth="1"/>
+    <col min="16" max="16" width="21.28515625" customWidth="1"/>
+    <col min="17" max="17" width="13.42578125" style="24" customWidth="1"/>
+    <col min="18" max="19" width="16.140625" customWidth="1"/>
+    <col min="20" max="21" width="27.42578125" customWidth="1"/>
+    <col min="22" max="23" width="18.42578125" customWidth="1"/>
+    <col min="24" max="25" width="12.28515625" customWidth="1"/>
+    <col min="26" max="27" width="20.28515625" customWidth="1"/>
+    <col min="28" max="28" width="15.140625" style="14" customWidth="1"/>
+    <col min="29" max="29" width="12.140625" style="14" customWidth="1"/>
+    <col min="30" max="30" width="14.42578125" customWidth="1"/>
+    <col min="31" max="31" width="17.42578125" customWidth="1"/>
+    <col min="32" max="32" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" s="3" customFormat="1">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:34" s="3" customFormat="1">
+      <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="N1" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="O1" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="P1" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="T1" s="31" t="s">
+      <c r="Q1" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="R1" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="S1" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="T1" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="U1" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="V1" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="W1" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="X1" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="AB1" s="2" t="s">
+      <c r="Y1" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="AC1" s="2" t="s">
+      <c r="Z1" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="AD1" s="2" t="s">
+      <c r="AA1" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="AE1" s="32" t="s">
+      <c r="AB1" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="AF1" s="32" t="s">
+      <c r="AC1" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="AG1" s="2" t="s">
+      <c r="AD1" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="AH1" s="2" t="s">
+      <c r="AE1" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="AI1" s="31" t="s">
+      <c r="AF1" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="AJ1" s="31" t="s">
+      <c r="AG1" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="AK1" s="31" t="s">
+      <c r="AH1" s="28" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:37" s="11" customFormat="1" ht="42.75">
-      <c r="A2" s="26" t="s">
+    <row r="2" spans="1:34" s="10" customFormat="1" ht="42.75">
+      <c r="A2" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="27" t="s">
+      <c r="C2" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="D2" s="29">
+      <c r="D2" s="26">
         <v>2019</v>
       </c>
-      <c r="E2" s="27" t="s">
+      <c r="E2" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="F2" s="26" t="s">
+      <c r="F2" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="G2" s="27" t="s">
+      <c r="G2" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="H2" s="30" t="s">
+      <c r="H2" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="I2" s="27" t="s">
+      <c r="I2" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="J2" s="27" t="s">
+      <c r="J2" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="K2" s="27">
+      <c r="K2" s="26">
         <v>2.68</v>
       </c>
-      <c r="L2" s="27">
+      <c r="L2" s="26">
         <v>260</v>
       </c>
-      <c r="M2" s="27" t="s">
+      <c r="M2" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="N2" s="30">
+      <c r="N2" s="25">
         <v>33</v>
       </c>
-      <c r="O2" s="30">
+      <c r="O2" s="25">
         <v>30</v>
       </c>
-      <c r="S2" s="33">
+      <c r="P2" s="29">
         <v>16.16</v>
       </c>
-      <c r="T2" s="33">
+      <c r="Q2" s="29">
         <v>2.74</v>
       </c>
-      <c r="U2" s="27" t="s">
+      <c r="R2" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="V2" s="27" t="s">
+      <c r="S2" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="W2" s="27">
+      <c r="T2" s="26">
         <v>16.170000000000002</v>
       </c>
-      <c r="X2" s="27">
+      <c r="U2" s="26">
         <v>1.89</v>
       </c>
-      <c r="Y2" s="27" t="s">
+      <c r="V2" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="Z2" s="27" t="s">
+      <c r="W2" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="AA2" s="26">
+      <c r="X2" s="25">
         <v>34</v>
       </c>
-      <c r="AB2" s="26">
+      <c r="Y2" s="25">
         <v>2.2000000000000002</v>
       </c>
-      <c r="AC2" s="26">
+      <c r="Z2" s="25">
         <v>33.9</v>
       </c>
-      <c r="AD2" s="26">
+      <c r="AA2" s="25">
         <v>2.2000000000000002</v>
       </c>
+      <c r="AB2" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="AC2" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="AD2" s="26" t="s">
+        <v>47</v>
+      </c>
       <c r="AE2" s="26" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="AF2" s="26" t="s">
-        <v>46</v>
-      </c>
-      <c r="AG2" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG2" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="AH2" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:34" s="10" customFormat="1" ht="42.75">
+      <c r="A3" s="25" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" s="26">
+        <v>2019</v>
+      </c>
+      <c r="E3" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="F3" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="G3" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="H3" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="I3" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="J3" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="K3" s="26">
+        <v>2.68</v>
+      </c>
+      <c r="L3" s="26">
+        <v>260</v>
+      </c>
+      <c r="M3" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="N3" s="25">
+        <v>25</v>
+      </c>
+      <c r="O3" s="25">
+        <v>15</v>
+      </c>
+      <c r="P3" s="29">
+        <v>15.47</v>
+      </c>
+      <c r="Q3" s="29">
+        <v>2.59</v>
+      </c>
+      <c r="R3" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="S3" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="T3" s="26">
+        <v>15.47</v>
+      </c>
+      <c r="U3" s="26">
+        <v>1.82</v>
+      </c>
+      <c r="V3" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="W3" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="X3" s="25">
+        <v>23.5</v>
+      </c>
+      <c r="Y3" s="25">
+        <v>0.86</v>
+      </c>
+      <c r="Z3" s="25">
+        <v>25.6</v>
+      </c>
+      <c r="AA3" s="25">
+        <v>0.97</v>
+      </c>
+      <c r="AB3" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="AC3" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="AD3" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="AH2" s="27" t="s">
-        <v>48</v>
-      </c>
-      <c r="AI2" s="27" t="s">
+      <c r="AE3" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="AF3" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="AJ2" s="27" t="s">
+      <c r="AG3" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="AK2" s="27">
+      <c r="AH3" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:37" s="11" customFormat="1" ht="42.75">
-      <c r="A3" s="26" t="s">
-        <v>49</v>
-      </c>
-      <c r="B3" s="27" t="s">
-        <v>50</v>
-      </c>
-      <c r="C3" s="27" t="s">
-        <v>36</v>
-      </c>
-      <c r="D3" s="29">
-        <v>2019</v>
-      </c>
-      <c r="E3" s="27" t="s">
-        <v>51</v>
-      </c>
-      <c r="F3" s="26" t="s">
-        <v>38</v>
-      </c>
-      <c r="G3" s="27" t="s">
-        <v>39</v>
-      </c>
-      <c r="H3" s="30" t="s">
-        <v>40</v>
-      </c>
-      <c r="I3" s="27" t="s">
-        <v>41</v>
-      </c>
-      <c r="J3" s="27" t="s">
+    <row r="4" spans="1:34" s="5" customFormat="1" ht="28.5">
+      <c r="A4" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="D4" s="26">
+        <v>2020</v>
+      </c>
+      <c r="E4" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="F4" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="G4" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="H4" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="I4" s="26" t="s">
+        <v>61</v>
+      </c>
+      <c r="J4" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="K4" s="26">
+        <v>14</v>
+      </c>
+      <c r="L4" s="26">
+        <v>600</v>
+      </c>
+      <c r="M4" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="N4" s="26">
+        <v>30</v>
+      </c>
+      <c r="O4" s="26">
+        <v>8</v>
+      </c>
+      <c r="P4" s="26">
+        <v>13.26</v>
+      </c>
+      <c r="Q4" s="26">
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="R4" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="S4" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="T4" s="26">
+        <v>15.16</v>
+      </c>
+      <c r="U4" s="26">
+        <v>4.5199999999999996</v>
+      </c>
+      <c r="V4" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="W4" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="X4" s="26">
+        <v>25.63</v>
+      </c>
+      <c r="Y4" s="26">
+        <v>4.24</v>
+      </c>
+      <c r="Z4" s="26">
+        <v>23.07</v>
+      </c>
+      <c r="AA4" s="26">
+        <v>4.72</v>
+      </c>
+      <c r="AB4" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="AC4" s="26" t="s">
+        <v>65</v>
+      </c>
+      <c r="AD4" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE4" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="AF4" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG4" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="AH4" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:34" s="10" customFormat="1" ht="57">
+      <c r="A5" s="27" t="s">
+        <v>66</v>
+      </c>
+      <c r="B5" s="26" t="s">
+        <v>67</v>
+      </c>
+      <c r="C5" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="D5" s="26">
+        <v>2008</v>
+      </c>
+      <c r="E5" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="G5" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="H5" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="I5" s="26" t="s">
+        <v>61</v>
+      </c>
+      <c r="J5" s="26" t="s">
+        <v>71</v>
+      </c>
+      <c r="K5" s="26">
+        <v>14</v>
+      </c>
+      <c r="L5" s="26">
+        <v>600</v>
+      </c>
+      <c r="M5" s="25" t="s">
+        <v>72</v>
+      </c>
+      <c r="N5" s="26">
+        <v>20</v>
+      </c>
+      <c r="O5" s="26">
+        <v>34</v>
+      </c>
+      <c r="P5" s="26">
+        <v>19.600000000000001</v>
+      </c>
+      <c r="Q5" s="26">
+        <v>3.8</v>
+      </c>
+      <c r="R5" s="26">
+        <v>11</v>
+      </c>
+      <c r="S5" s="26">
+        <v>3.9</v>
+      </c>
+      <c r="T5" s="26">
+        <v>22.6</v>
+      </c>
+      <c r="U5" s="26">
+        <v>5.6</v>
+      </c>
+      <c r="V5" s="26">
+        <v>10</v>
+      </c>
+      <c r="W5" s="26">
+        <v>3.1</v>
+      </c>
+      <c r="X5" s="26">
+        <v>43.8</v>
+      </c>
+      <c r="Y5" s="26">
+        <v>11.2</v>
+      </c>
+      <c r="Z5" s="26">
+        <v>44.6</v>
+      </c>
+      <c r="AA5" s="26">
+        <v>15.2</v>
+      </c>
+      <c r="AB5" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="AC5" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="AD5" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="AE5" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="AF5" s="25">
+        <v>671</v>
+      </c>
+      <c r="AG5" s="25">
+        <v>572</v>
+      </c>
+      <c r="AH5" s="25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:34" s="5" customFormat="1" ht="57">
+      <c r="A6" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="B6" s="26" t="s">
+        <v>76</v>
+      </c>
+      <c r="C6" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="D6" s="26">
+        <v>2010</v>
+      </c>
+      <c r="E6" s="26" t="s">
+        <v>78</v>
+      </c>
+      <c r="F6" s="26" t="s">
+        <v>79</v>
+      </c>
+      <c r="G6" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="H6" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="I6" s="26" t="s">
+        <v>61</v>
+      </c>
+      <c r="J6" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="K3" s="27">
-        <v>2.68</v>
-      </c>
-      <c r="L3" s="27">
-        <v>260</v>
-      </c>
-      <c r="M3" s="27" t="s">
-        <v>43</v>
-      </c>
-      <c r="N3" s="30">
-        <v>25</v>
-      </c>
-      <c r="O3" s="30">
-        <v>15</v>
-      </c>
-      <c r="S3" s="33">
-        <v>15.47</v>
-      </c>
-      <c r="T3" s="33">
-        <v>2.59</v>
-      </c>
-      <c r="U3" s="27" t="s">
-        <v>44</v>
-      </c>
-      <c r="V3" s="27" t="s">
-        <v>44</v>
-      </c>
-      <c r="W3" s="27">
-        <v>15.47</v>
-      </c>
-      <c r="X3" s="27">
-        <v>1.82</v>
-      </c>
-      <c r="Y3" s="27" t="s">
-        <v>44</v>
-      </c>
-      <c r="Z3" s="27" t="s">
-        <v>44</v>
-      </c>
-      <c r="AA3" s="26">
-        <v>23.5</v>
-      </c>
-      <c r="AB3" s="26">
-        <v>0.86</v>
-      </c>
-      <c r="AC3" s="26">
-        <v>25.6</v>
-      </c>
-      <c r="AD3" s="26">
-        <v>0.97</v>
-      </c>
-      <c r="AE3" s="27" t="s">
+      <c r="K6" s="26">
+        <v>14</v>
+      </c>
+      <c r="L6" s="26">
+        <v>600</v>
+      </c>
+      <c r="M6" s="25" t="s">
+        <v>72</v>
+      </c>
+      <c r="N6" s="26">
+        <v>23</v>
+      </c>
+      <c r="O6" s="26">
+        <v>23</v>
+      </c>
+      <c r="P6" s="26">
+        <v>20.5</v>
+      </c>
+      <c r="Q6" s="26">
+        <v>3.4</v>
+      </c>
+      <c r="R6" s="26">
+        <v>10.9</v>
+      </c>
+      <c r="S6" s="26">
+        <v>3.2</v>
+      </c>
+      <c r="T6" s="26">
+        <v>22.6</v>
+      </c>
+      <c r="U6" s="26">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="V6" s="26">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="W6" s="26">
+        <v>3.4</v>
+      </c>
+      <c r="X6" s="26">
+        <v>47</v>
+      </c>
+      <c r="Y6" s="26">
+        <v>16.899999999999999</v>
+      </c>
+      <c r="Z6" s="26">
+        <v>44.9</v>
+      </c>
+      <c r="AA6" s="33">
+        <v>13.6</v>
+      </c>
+      <c r="AB6" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="AC6" s="26" t="s">
+        <v>81</v>
+      </c>
+      <c r="AD6" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="AE6" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="AF6" s="26">
+        <v>656</v>
+      </c>
+      <c r="AG6" s="26">
+        <v>537</v>
+      </c>
+      <c r="AH6" s="26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:34" s="10" customFormat="1" ht="42.75">
+      <c r="A7" s="25" t="s">
+        <v>82</v>
+      </c>
+      <c r="B7" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="C7" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="D7" s="26">
+        <v>2014</v>
+      </c>
+      <c r="E7" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="F7" s="26">
         <v>52</v>
       </c>
-      <c r="AF3" s="26" t="s">
-        <v>53</v>
-      </c>
-      <c r="AG3" s="27" t="s">
+      <c r="G7" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="H7" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="I7" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="J7" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="K7" s="26">
+        <v>2.4</v>
+      </c>
+      <c r="L7" s="26">
+        <v>38.4</v>
+      </c>
+      <c r="M7" s="25" t="s">
+        <v>72</v>
+      </c>
+      <c r="N7" s="26">
+        <v>52</v>
+      </c>
+      <c r="O7" s="26">
+        <v>52</v>
+      </c>
+      <c r="P7" s="26">
+        <v>9.6</v>
+      </c>
+      <c r="Q7" s="26">
+        <v>2.36</v>
+      </c>
+      <c r="R7" s="26">
+        <v>13.44</v>
+      </c>
+      <c r="S7" s="26">
+        <v>3.37</v>
+      </c>
+      <c r="T7" s="26">
+        <v>10.89</v>
+      </c>
+      <c r="U7" s="26">
+        <v>2.37</v>
+      </c>
+      <c r="V7" s="26">
+        <v>14.21</v>
+      </c>
+      <c r="W7" s="26">
+        <v>3.5</v>
+      </c>
+      <c r="X7" s="26">
+        <v>34.6</v>
+      </c>
+      <c r="Y7" s="26">
+        <v>13.7</v>
+      </c>
+      <c r="Z7" s="26">
+        <v>35.1</v>
+      </c>
+      <c r="AA7" s="26">
+        <v>13.3</v>
+      </c>
+      <c r="AB7" s="26" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC7" s="26" t="s">
+        <v>87</v>
+      </c>
+      <c r="AD7" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="AH3" s="27" t="s">
-        <v>54</v>
-      </c>
-      <c r="AI3" s="26" t="s">
-        <v>44</v>
-      </c>
-      <c r="AJ3" s="26" t="s">
-        <v>44</v>
-      </c>
-      <c r="AK3" s="26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:37" s="6" customFormat="1" ht="28.5">
-      <c r="A4" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C4" s="27" t="s">
-        <v>57</v>
-      </c>
-      <c r="D4" s="5">
-        <v>2020</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="I4" s="27" t="s">
-        <v>61</v>
-      </c>
-      <c r="J4" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="K4" s="5">
-        <v>14</v>
-      </c>
-      <c r="L4" s="5">
-        <v>600</v>
-      </c>
-      <c r="M4" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="N4" s="5">
-        <v>30</v>
-      </c>
-      <c r="O4" s="5">
-        <v>8</v>
-      </c>
-      <c r="S4" s="5">
-        <v>13.26</v>
-      </c>
-      <c r="T4" s="27">
-        <v>2.5499999999999998</v>
-      </c>
-      <c r="U4" s="27" t="s">
-        <v>44</v>
-      </c>
-      <c r="V4" s="27" t="s">
-        <v>63</v>
-      </c>
-      <c r="W4" s="27">
-        <v>15.16</v>
-      </c>
-      <c r="X4" s="27">
-        <v>4.5199999999999996</v>
-      </c>
-      <c r="Y4" s="27" t="s">
-        <v>44</v>
-      </c>
-      <c r="Z4" s="27" t="s">
-        <v>44</v>
-      </c>
-      <c r="AA4" s="27">
-        <v>25.63</v>
-      </c>
-      <c r="AB4" s="27">
-        <v>4.24</v>
-      </c>
-      <c r="AC4" s="27">
-        <v>23.07</v>
-      </c>
-      <c r="AD4" s="27">
-        <v>4.72</v>
-      </c>
-      <c r="AE4" s="34" t="s">
-        <v>64</v>
-      </c>
-      <c r="AF4" s="34" t="s">
-        <v>65</v>
-      </c>
-      <c r="AG4" s="27" t="s">
-        <v>54</v>
-      </c>
-      <c r="AH4" s="27" t="s">
-        <v>54</v>
-      </c>
-      <c r="AI4" s="27" t="s">
-        <v>44</v>
-      </c>
-      <c r="AJ4" s="27" t="s">
-        <v>44</v>
-      </c>
-      <c r="AK4" s="27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:37" s="11" customFormat="1" ht="57">
-      <c r="A5" s="28" t="s">
-        <v>66</v>
-      </c>
-      <c r="B5" s="27" t="s">
-        <v>67</v>
-      </c>
-      <c r="C5" s="27" t="s">
-        <v>68</v>
-      </c>
-      <c r="D5" s="29">
-        <v>2008</v>
-      </c>
-      <c r="E5" s="27" t="s">
-        <v>37</v>
-      </c>
-      <c r="F5" s="27" t="s">
-        <v>69</v>
-      </c>
-      <c r="G5" s="26" t="s">
-        <v>70</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="I5" s="27" t="s">
-        <v>61</v>
-      </c>
-      <c r="J5" s="27" t="s">
-        <v>71</v>
-      </c>
-      <c r="K5" s="27">
-        <v>14</v>
-      </c>
-      <c r="L5" s="27">
-        <v>600</v>
-      </c>
-      <c r="M5" s="26" t="s">
-        <v>72</v>
-      </c>
-      <c r="N5" s="29">
-        <v>20</v>
-      </c>
-      <c r="O5" s="29">
-        <v>34</v>
-      </c>
-      <c r="S5" s="27">
-        <v>19.600000000000001</v>
-      </c>
-      <c r="T5" s="27">
-        <v>3.8</v>
-      </c>
-      <c r="U5" s="27">
-        <v>11</v>
-      </c>
-      <c r="V5" s="27">
-        <v>3.9</v>
-      </c>
-      <c r="W5" s="27">
-        <v>22.6</v>
-      </c>
-      <c r="X5" s="27">
-        <v>5.6</v>
-      </c>
-      <c r="Y5" s="27">
-        <v>10</v>
-      </c>
-      <c r="Z5" s="27">
-        <v>3.1</v>
-      </c>
-      <c r="AA5" s="27">
-        <v>43.8</v>
-      </c>
-      <c r="AB5" s="27">
-        <v>11.2</v>
-      </c>
-      <c r="AC5" s="27">
-        <v>44.6</v>
-      </c>
-      <c r="AD5" s="27">
-        <v>15.2</v>
-      </c>
-      <c r="AE5" s="27" t="s">
-        <v>73</v>
-      </c>
-      <c r="AF5" s="27" t="s">
-        <v>74</v>
-      </c>
-      <c r="AG5" s="27" t="s">
+      <c r="AE7" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="AH5" s="27" t="s">
-        <v>54</v>
-      </c>
-      <c r="AI5" s="26">
-        <v>671</v>
-      </c>
-      <c r="AJ5" s="26">
-        <v>572</v>
-      </c>
-      <c r="AK5" s="26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:37" s="6" customFormat="1" ht="57">
-      <c r="A6" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="C6" s="27" t="s">
-        <v>77</v>
-      </c>
-      <c r="D6" s="5">
-        <v>2010</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="I6" s="27" t="s">
-        <v>61</v>
-      </c>
-      <c r="J6" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="K6" s="5">
-        <v>14</v>
-      </c>
-      <c r="L6" s="5">
-        <v>600</v>
-      </c>
-      <c r="M6" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="N6" s="5">
-        <v>23</v>
-      </c>
-      <c r="O6" s="5">
-        <v>23</v>
-      </c>
-      <c r="S6" s="5">
-        <v>20.5</v>
-      </c>
-      <c r="T6" s="27">
-        <v>3.4</v>
-      </c>
-      <c r="U6" s="5">
-        <v>10.9</v>
-      </c>
-      <c r="V6" s="5">
-        <v>3.2</v>
-      </c>
-      <c r="W6" s="5">
-        <v>22.6</v>
-      </c>
-      <c r="X6" s="5">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="Y6" s="5">
-        <v>9.8000000000000007</v>
-      </c>
-      <c r="Z6" s="5">
-        <v>3.4</v>
-      </c>
-      <c r="AA6" s="5">
-        <v>47</v>
-      </c>
-      <c r="AB6" s="29">
-        <v>16.899999999999999</v>
-      </c>
-      <c r="AC6" s="5">
-        <v>44.9</v>
-      </c>
-      <c r="AD6" s="35">
-        <v>13.6</v>
-      </c>
-      <c r="AE6" s="34" t="s">
-        <v>80</v>
-      </c>
-      <c r="AF6" s="34" t="s">
-        <v>81</v>
-      </c>
-      <c r="AG6" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="AH6" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="AI6" s="27">
-        <v>656</v>
-      </c>
-      <c r="AJ6" s="27">
-        <v>537</v>
-      </c>
-      <c r="AK6" s="27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:37" s="11" customFormat="1" ht="42.75">
-      <c r="A7" s="26" t="s">
-        <v>82</v>
-      </c>
-      <c r="B7" s="27" t="s">
-        <v>83</v>
-      </c>
-      <c r="C7" s="27" t="s">
-        <v>84</v>
-      </c>
-      <c r="D7" s="29">
-        <v>2014</v>
-      </c>
-      <c r="E7" s="27" t="s">
-        <v>37</v>
-      </c>
-      <c r="F7" s="29">
-        <v>52</v>
-      </c>
-      <c r="G7" s="26" t="s">
-        <v>85</v>
-      </c>
-      <c r="H7" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="I7" s="27" t="s">
-        <v>86</v>
-      </c>
-      <c r="J7" s="27" t="s">
-        <v>42</v>
-      </c>
-      <c r="K7" s="27">
-        <v>2.4</v>
-      </c>
-      <c r="L7" s="27">
-        <v>38.4</v>
-      </c>
-      <c r="M7" s="26" t="s">
-        <v>72</v>
-      </c>
-      <c r="N7" s="29">
-        <v>52</v>
-      </c>
-      <c r="O7" s="29">
-        <v>52</v>
-      </c>
-      <c r="S7" s="27">
-        <v>9.6</v>
-      </c>
-      <c r="T7" s="27">
-        <v>2.36</v>
-      </c>
-      <c r="U7" s="27">
-        <v>13.44</v>
-      </c>
-      <c r="V7" s="27">
-        <v>3.37</v>
-      </c>
-      <c r="W7" s="27">
-        <v>10.89</v>
-      </c>
-      <c r="X7" s="27">
-        <v>2.37</v>
-      </c>
-      <c r="Y7" s="27">
-        <v>14.21</v>
-      </c>
-      <c r="Z7" s="27">
-        <v>3.5</v>
-      </c>
-      <c r="AA7" s="27">
-        <v>34.6</v>
-      </c>
-      <c r="AB7" s="27">
-        <v>13.7</v>
-      </c>
-      <c r="AC7" s="27">
-        <v>35.1</v>
-      </c>
-      <c r="AD7" s="27">
-        <v>13.3</v>
-      </c>
-      <c r="AE7" s="27" t="s">
-        <v>87</v>
-      </c>
-      <c r="AF7" s="27" t="s">
-        <v>87</v>
-      </c>
-      <c r="AG7" s="27" t="s">
-        <v>47</v>
-      </c>
-      <c r="AH7" s="27" t="s">
-        <v>47</v>
-      </c>
-      <c r="AI7" s="27">
+      <c r="AF7" s="26">
         <v>596.20000000000005</v>
       </c>
-      <c r="AJ7" s="27">
+      <c r="AG7" s="26">
         <v>556.20000000000005</v>
       </c>
-      <c r="AK7" s="27">
+      <c r="AH7" s="26">
         <v>1</v>
       </c>
     </row>
@@ -1832,7 +1822,7 @@
       <c r="N1" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="O1" s="24" t="s">
+      <c r="O1" s="23" t="s">
         <v>16</v>
       </c>
       <c r="P1" s="3" t="s">
@@ -1850,10 +1840,10 @@
       <c r="T1" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="U1" s="14" t="s">
+      <c r="U1" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="V1" s="14" t="s">
+      <c r="V1" s="13" t="s">
         <v>28</v>
       </c>
       <c r="W1" s="3" t="s">
@@ -1869,188 +1859,188 @@
         <v>103</v>
       </c>
     </row>
-    <row r="2" spans="1:26" s="8" customFormat="1" ht="78.75" customHeight="1">
-      <c r="A2" s="9" t="s">
+    <row r="2" spans="1:26" s="7" customFormat="1" ht="78.75" customHeight="1">
+      <c r="A2" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="C2" s="7">
+      <c r="C2" s="6">
         <v>2017</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="H2" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="I2" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="J2" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="K2" s="8" t="s">
+      <c r="K2" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="M2" s="10"/>
-      <c r="O2" s="12"/>
-      <c r="P2" s="12"/>
-      <c r="Q2" s="12"/>
-      <c r="R2" s="12"/>
-      <c r="S2" s="12"/>
-      <c r="T2" s="12"/>
-      <c r="U2" s="16"/>
-      <c r="V2" s="16"/>
-      <c r="W2" s="12"/>
-      <c r="X2" s="12"/>
+      <c r="M2" s="9"/>
+      <c r="O2" s="11"/>
+      <c r="P2" s="11"/>
+      <c r="Q2" s="11"/>
+      <c r="R2" s="11"/>
+      <c r="S2" s="11"/>
+      <c r="T2" s="11"/>
+      <c r="U2" s="15"/>
+      <c r="V2" s="15"/>
+      <c r="W2" s="11"/>
+      <c r="X2" s="11"/>
     </row>
-    <row r="3" spans="1:26" s="8" customFormat="1" ht="71.25" customHeight="1">
-      <c r="A3" s="9" t="s">
+    <row r="3" spans="1:26" s="7" customFormat="1" ht="71.25" customHeight="1">
+      <c r="A3" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C3" s="6">
         <v>2020</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="E3" s="7">
+      <c r="E3" s="6">
         <v>11</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="G3" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="H3" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="I3" s="7" t="s">
+      <c r="I3" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="J3" s="7" t="s">
+      <c r="J3" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="K3" s="8" t="s">
+      <c r="K3" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="M3" s="10"/>
-      <c r="O3" s="12"/>
-      <c r="P3" s="12"/>
-      <c r="Q3" s="12"/>
-      <c r="R3" s="12"/>
-      <c r="S3" s="12"/>
-      <c r="T3" s="12"/>
-      <c r="U3" s="16"/>
-      <c r="V3" s="16"/>
-      <c r="W3" s="12"/>
-      <c r="X3" s="12"/>
+      <c r="M3" s="9"/>
+      <c r="O3" s="11"/>
+      <c r="P3" s="11"/>
+      <c r="Q3" s="11"/>
+      <c r="R3" s="11"/>
+      <c r="S3" s="11"/>
+      <c r="T3" s="11"/>
+      <c r="U3" s="15"/>
+      <c r="V3" s="15"/>
+      <c r="W3" s="11"/>
+      <c r="X3" s="11"/>
     </row>
-    <row r="4" spans="1:26" s="10" customFormat="1" ht="78.75" customHeight="1">
-      <c r="A4" s="9" t="s">
+    <row r="4" spans="1:26" s="9" customFormat="1" ht="78.75" customHeight="1">
+      <c r="A4" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="C4" s="9">
+      <c r="C4" s="8">
         <v>2013</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="E4" s="9">
+      <c r="E4" s="8">
         <v>5</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="F4" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9" t="s">
+      <c r="G4" s="8"/>
+      <c r="H4" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="I4" s="9" t="s">
+      <c r="I4" s="8" t="s">
         <v>125</v>
       </c>
-      <c r="J4" s="9" t="s">
+      <c r="J4" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="K4" s="10" t="s">
+      <c r="K4" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="O4" s="13"/>
-      <c r="P4" s="13"/>
-      <c r="Q4" s="13"/>
-      <c r="R4" s="13"/>
-      <c r="S4" s="13"/>
-      <c r="T4" s="13"/>
-      <c r="U4" s="17"/>
-      <c r="V4" s="17"/>
-      <c r="W4" s="13"/>
-      <c r="X4" s="13"/>
+      <c r="O4" s="12"/>
+      <c r="P4" s="12"/>
+      <c r="Q4" s="12"/>
+      <c r="R4" s="12"/>
+      <c r="S4" s="12"/>
+      <c r="T4" s="12"/>
+      <c r="U4" s="16"/>
+      <c r="V4" s="16"/>
+      <c r="W4" s="12"/>
+      <c r="X4" s="12"/>
     </row>
-    <row r="5" spans="1:26" s="20" customFormat="1" ht="78.75" customHeight="1">
-      <c r="A5" s="18" t="s">
+    <row r="5" spans="1:26" s="19" customFormat="1" ht="78.75" customHeight="1">
+      <c r="A5" s="17" t="s">
         <v>126</v>
       </c>
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="18" t="s">
         <v>127</v>
       </c>
-      <c r="C5" s="19">
+      <c r="C5" s="18">
         <v>2020</v>
       </c>
-      <c r="D5" s="19" t="s">
+      <c r="D5" s="18" t="s">
         <v>128</v>
       </c>
-      <c r="E5" s="19" t="s">
+      <c r="E5" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="F5" s="19" t="s">
+      <c r="F5" s="18" t="s">
         <v>130</v>
       </c>
-      <c r="G5" s="19" t="s">
+      <c r="G5" s="18" t="s">
         <v>117</v>
       </c>
-      <c r="H5" s="19" t="s">
+      <c r="H5" s="18" t="s">
         <v>110</v>
       </c>
-      <c r="I5" s="19" t="s">
+      <c r="I5" s="18" t="s">
         <v>131</v>
       </c>
-      <c r="J5" s="19" t="s">
+      <c r="J5" s="18" t="s">
         <v>132</v>
       </c>
-      <c r="K5" s="20" t="s">
+      <c r="K5" s="19" t="s">
         <v>133</v>
       </c>
-      <c r="M5" s="23" t="s">
+      <c r="M5" s="22" t="s">
         <v>134</v>
       </c>
-      <c r="O5" s="21"/>
-      <c r="P5" s="21"/>
-      <c r="R5" s="21"/>
-      <c r="S5" s="21"/>
-      <c r="T5" s="21"/>
-      <c r="U5" s="22"/>
-      <c r="V5" s="22"/>
-      <c r="W5" s="21"/>
-      <c r="X5" s="21"/>
-      <c r="Y5" s="23" t="s">
+      <c r="O5" s="20"/>
+      <c r="P5" s="20"/>
+      <c r="R5" s="20"/>
+      <c r="S5" s="20"/>
+      <c r="T5" s="20"/>
+      <c r="U5" s="21"/>
+      <c r="V5" s="21"/>
+      <c r="W5" s="20"/>
+      <c r="X5" s="20"/>
+      <c r="Y5" s="22" t="s">
         <v>135</v>
       </c>
     </row>
@@ -2087,20 +2077,20 @@
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="37" t="s">
+      <c r="B1" s="31" t="s">
         <v>136</v>
       </c>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37" t="s">
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31" t="s">
         <v>137</v>
       </c>
-      <c r="G1" s="37"/>
-      <c r="H1" s="38" t="s">
+      <c r="G1" s="31"/>
+      <c r="H1" s="32" t="s">
         <v>138</v>
       </c>
-      <c r="I1" s="38"/>
+      <c r="I1" s="32"/>
       <c r="J1" t="s">
         <v>139</v>
       </c>
@@ -2125,7 +2115,7 @@
       <c r="F2" t="s">
         <v>145</v>
       </c>
-      <c r="G2" s="36" t="s">
+      <c r="G2" s="30" t="s">
         <v>146</v>
       </c>
       <c r="H2" t="s">
@@ -2136,7 +2126,7 @@
       </c>
     </row>
     <row r="3" spans="1:11">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="26" t="s">
         <v>83</v>
       </c>
       <c r="B3" t="s">
@@ -2171,7 +2161,7 @@
       </c>
     </row>
     <row r="4" spans="1:11">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="26" t="s">
         <v>35</v>
       </c>
       <c r="B4" t="s">
@@ -2200,7 +2190,7 @@
       </c>
     </row>
     <row r="5" spans="1:11">
-      <c r="A5" s="27" t="s">
+      <c r="A5" s="26" t="s">
         <v>50</v>
       </c>
       <c r="B5" t="s">
@@ -2229,7 +2219,7 @@
       </c>
     </row>
     <row r="6" spans="1:11">
-      <c r="A6" s="27" t="s">
+      <c r="A6" s="26" t="s">
         <v>67</v>
       </c>
       <c r="B6" t="s">
@@ -2258,7 +2248,7 @@
       </c>
     </row>
     <row r="7" spans="1:11">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="4" t="s">
         <v>151</v>
       </c>
       <c r="B7" t="s">
@@ -2287,7 +2277,7 @@
       </c>
     </row>
     <row r="8" spans="1:11">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="4" t="s">
         <v>76</v>
       </c>
       <c r="B8" t="s">
@@ -2316,7 +2306,7 @@
       </c>
     </row>
     <row r="9" spans="1:11">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="4" t="s">
         <v>56</v>
       </c>
       <c r="B9" t="s">
@@ -2566,12 +2556,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -2580,14 +2564,20 @@
 </FormTemplates>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8ECA79A9-07DD-4BBF-BB33-7E4654FD1849}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{14283630-5988-43E0-B4F4-4C59212AE6BF}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9080AD7B-1842-4234-9D7C-AFD30CCC1256}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9080AD7B-1842-4234-9D7C-AFD30CCC1256}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{14283630-5988-43E0-B4F4-4C59212AE6BF}"/>
 </file>
</xml_diff>